<commit_message>
FileCounter: Remove and replace test with a ScannerIntegrationFunTest
This allows for an integration test for the scanner, but removes
the superfluous file counter scanner, now that fileCount is removed.

Signed-off-by: Stephanie Neubauer <Stephanie.Neubauer@bosch.io>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/dummy-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/dummy-expected-scan-report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sse1be\Development\GitHub\oss-review-toolkit\ort\reporter\src\funTest\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nes1wa3\OneDrive - Robert Bosch GmbH\Documents\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5F3D68-2701-4389-8F27-EFE65A4E6A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E3E37C-B676-4D0E-ADE3-2419D569F979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -241,25 +241,25 @@
     </r>
   </si>
   <si>
+    <t>ResolvedLicense(license=EPL-1.0, originalDeclaredLicenses=[Eclipse Public License 1.0], originalExpressions={DECLARED=[EPL-1.0]}, locations=[])</t>
+  </si>
+  <si>
+    <t>ResolvedLicense(license=Apache-2.0, originalDeclaredLicenses=[Apache License, Version 2.0], originalExpressions={DECLARED=[Apache-2.0]}, locations=[])</t>
+  </si>
+  <si>
+    <t>ResolvedLicense(license=BSD-3-Clause, originalDeclaredLicenses=[New BSD License], originalExpressions={DECLARED=[BSD-3-Clause]}, locations=[])</t>
+  </si>
+  <si>
+    <t>Unknown time [ERROR]: Dummy - Could not download 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': DownloadException: Download failed for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
+Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
+Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0
-  Unknown time [ERROR]: FileCounter - Could not download 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': DownloadException: Download failed for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
+  Unknown time [ERROR]: Dummy - Could not download 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': DownloadException: Download failed for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
 Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
 Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
 </t>
-  </si>
-  <si>
-    <t>Unknown time [ERROR]: FileCounter - Could not download 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': DownloadException: Download failed for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
-Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
-Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.</t>
-  </si>
-  <si>
-    <t>ResolvedLicense(license=EPL-1.0, originalDeclaredLicenses=[Eclipse Public License 1.0], originalExpressions={DECLARED=[EPL-1.0]}, locations=[])</t>
-  </si>
-  <si>
-    <t>ResolvedLicense(license=Apache-2.0, originalDeclaredLicenses=[Apache License, Version 2.0], originalExpressions={DECLARED=[Apache-2.0]}, locations=[])</t>
-  </si>
-  <si>
-    <t>ResolvedLicense(license=BSD-3-Clause, originalDeclaredLicenses=[New BSD License], originalExpressions={DECLARED=[BSD-3-Clause]}, locations=[])</t>
   </si>
 </sst>
 </file>
@@ -346,14 +346,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,11 +672,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,25 +692,25 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -721,49 +721,49 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -802,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,11 +903,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,25 +924,25 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -953,49 +953,49 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -1032,7 +1032,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1042,8 +1042,8 @@
       <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>35</v>
+      <c r="C12" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -1062,8 +1062,8 @@
       <c r="B13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>36</v>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1082,8 +1082,8 @@
       <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>36</v>
+      <c r="C14" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -1102,8 +1102,8 @@
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>37</v>
+      <c r="C15" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
ExcelReporter: Align showing declared with showing detected licenses
For detected licenses only the license expression is shown, while for
declared licenses the whole `ResolvedLicense` is shown. Align that by
showing only the expression of detected licenses.

Signed-off-by: Frank Viernau <frank.viernau@here.com>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/dummy-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/dummy-expected-scan-report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nes1wa3\OneDrive - Robert Bosch GmbH\Documents\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sse1be\Development\GitHub\oss-review-toolkit\ort\reporter\src\funTest\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E3E37C-B676-4D0E-ADE3-2419D569F979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C74F47B-82FB-4CA6-BBC9-0E337D1AD8D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6915" yWindow="3555" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -241,15 +241,6 @@
     </r>
   </si>
   <si>
-    <t>ResolvedLicense(license=EPL-1.0, originalDeclaredLicenses=[Eclipse Public License 1.0], originalExpressions={DECLARED=[EPL-1.0]}, locations=[])</t>
-  </si>
-  <si>
-    <t>ResolvedLicense(license=Apache-2.0, originalDeclaredLicenses=[Apache License, Version 2.0], originalExpressions={DECLARED=[Apache-2.0]}, locations=[])</t>
-  </si>
-  <si>
-    <t>ResolvedLicense(license=BSD-3-Clause, originalDeclaredLicenses=[New BSD License], originalExpressions={DECLARED=[BSD-3-Clause]}, locations=[])</t>
-  </si>
-  <si>
     <t>Unknown time [ERROR]: Dummy - Could not download 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': DownloadException: Download failed for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
 Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
 Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.</t>
@@ -260,6 +251,15 @@
 Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
 Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
 </t>
+  </si>
+  <si>
+    <t>EPL-1.0</t>
+  </si>
+  <si>
+    <t>Apache-2.0</t>
+  </si>
+  <si>
+    <t>BSD-3-Clause</t>
   </si>
 </sst>
 </file>
@@ -358,7 +358,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -672,14 +672,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
@@ -802,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -903,14 +903,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -1032,7 +1032,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1043,7 +1043,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -1063,7 +1063,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -1083,7 +1083,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -1103,7 +1103,7 @@
         <v>31</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
ScannerIntegrationFunTest: Use the experimental scanner
Change the test to use the experimental scanner to prepare removing the
legacy scanner. As the experimental scanner does not support the
calculation of the package verification code, create a list of fake
license findings instead to verify that the correct source code was
scanned.

Signed-off-by: Martin Nonnenmacher <martin.nonnenmacher@bosch.io>
</commit_message>
<xml_diff>
--- a/reporter/src/funTest/assets/dummy-expected-scan-report.xlsx
+++ b/reporter/src/funTest/assets/dummy-expected-scan-report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sse1be\Development\GitHub\oss-review-toolkit\ort\reporter\src\funTest\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Development\GitHub\oss-review-toolkit\ort\reporter\src\funTest\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C74F47B-82FB-4CA6-BBC9-0E337D1AD8D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D26FE1-AF51-436C-895D-BDB2398FE3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="3555" windowWidth="28800" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6135" yWindow="1740" windowWidth="28800" windowHeight="18630" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
   <si>
     <t>Project:</t>
   </si>
@@ -141,6 +141,15 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
       </rPr>
+      <t>NONE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t>Maven:org.apache.commons:commons-lang3:3.5</t>
     </r>
   </si>
@@ -241,32 +250,23 @@
     </r>
   </si>
   <si>
-    <t>Unknown time [ERROR]: Dummy - Could not download 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': DownloadException: Download failed for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
-Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
-Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0
-  Unknown time [ERROR]: Dummy - Could not download 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': DownloadException: Download failed for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
-Suppressed: DownloadException: No VCS URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'. Please make sure the published POM file includes the SCM connection, see: https://docs.gradle.org/current/userguide/publishing_maven.html#sec:modifying_the_generated_pom
-Suppressed: DownloadException: No source artifact URL provided for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0'.
+  Unknown time [ERROR]: scanner - Could not resolve provenance for package 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': IOException: Could not resolve provenance for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0' for source code origins [VCS, ARTIFACT].
+Resolution of VCS failed with:
+URISyntaxException: Cannot parse Git URI-ish: The uri was empty or null
 </t>
   </si>
   <si>
-    <t>EPL-1.0</t>
-  </si>
-  <si>
-    <t>Apache-2.0</t>
-  </si>
-  <si>
-    <t>BSD-3-Clause</t>
+    <t>Unknown time [ERROR]: scanner - Could not resolve provenance for package 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0': IOException: Could not resolve provenance for 'Gradle:org.ossreviewtoolkit.gradle.example:lib:1.0.0' for source code origins [VCS, ARTIFACT].
+Resolution of VCS failed with:
+URISyntaxException: Cannot parse Git URI-ish: The uri was empty or null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -329,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -343,22 +343,19 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -374,7 +371,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -676,96 +673,96 @@
       <pane xSplit="1" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="229.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="253.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -785,7 +782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -801,11 +798,11 @@
       <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -816,7 +813,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>8</v>
@@ -825,38 +822,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="75" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>8</v>
@@ -865,18 +862,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="45" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>8</v>
@@ -904,100 +901,100 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="10" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="102" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="229.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="252.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -1017,7 +1014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1031,22 +1028,22 @@
       <c r="E11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F11" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>8</v>
@@ -1055,58 +1052,58 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" customHeight="1">
       <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>37</v>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>8</v>

</xml_diff>